<commit_message>
Add SQL script to create database schema for employee benefits project
</commit_message>
<xml_diff>
--- a/docs/dictionnaire_des_donnees.xlsx
+++ b/docs/dictionnaire_des_donnees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maeva\Documents\OpenClassRoom\P12 - Gérer un projet d'infrastructure\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF67A220-FAD9-42A8-9C31-DB5AE03C4C93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AEEC54-7E31-4B1C-BBEC-6434A4A4D98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21710" yWindow="-110" windowWidth="21820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21710" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employes" sheetId="1" r:id="rId1"/>
@@ -368,10 +368,10 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -654,7 +654,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
@@ -669,14 +669,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -700,22 +700,22 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -873,14 +873,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -904,22 +904,22 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -988,14 +988,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1019,22 +1019,22 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1093,7 +1093,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1107,14 +1107,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1138,22 +1138,22 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -1263,8 +1263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9ABC34-4599-40B9-932D-82F7CF5DB92D}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1278,14 +1278,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
@@ -1309,22 +1309,22 @@
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="7"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">

</xml_diff>

<commit_message>
Add get_distance_google.py script for distance calculation
</commit_message>
<xml_diff>
--- a/docs/dictionnaire_des_donnees.xlsx
+++ b/docs/dictionnaire_des_donnees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maeva\Documents\OpenClassRoom\P12 - Gérer un projet d'infrastructure\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84AEEC54-7E31-4B1C-BBEC-6434A4A4D98F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D4D01E-903A-4819-8BB8-6007CE314A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21710" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21710" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employes" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="83">
   <si>
     <t>CHAMPS</t>
   </si>
@@ -75,9 +75,6 @@
   </si>
   <si>
     <t>nb_jours_cp</t>
-  </si>
-  <si>
-    <t>adresse</t>
   </si>
   <si>
     <t>mode_deplacement</t>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>Sport pratiqué régulièrement par l'employé</t>
+  </si>
+  <si>
+    <t>adresse_domicile</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -372,6 +372,9 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -655,7 +658,7 @@
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+      <selection activeCell="A13" sqref="A13:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -670,7 +673,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -704,16 +707,16 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -722,10 +725,10 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -733,10 +736,10 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -744,13 +747,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -758,10 +761,10 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -769,24 +772,24 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
       <c r="C10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -794,10 +797,10 @@
         <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -805,43 +808,43 @@
         <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>82</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="3" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>80</v>
+      </c>
+      <c r="B15" t="s">
         <v>81</v>
       </c>
-      <c r="B15" t="s">
-        <v>82</v>
-      </c>
       <c r="C15" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -856,10 +859,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89487438-E9F9-4E4A-99B5-90E8A4C27D7E}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -874,7 +877,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -908,56 +911,70 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="F4" s="6"/>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F6" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="B7" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>39</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D7" t="s">
         <v>41</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>17</v>
+      <c r="C8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -989,7 +1006,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1023,57 +1040,57 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -1108,7 +1125,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1139,19 +1156,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>54</v>
-      </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6"/>
     </row>
@@ -1160,94 +1177,94 @@
         <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="C9" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>64</v>
-      </c>
       <c r="C11" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -1263,7 +1280,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA9ABC34-4599-40B9-932D-82F7CF5DB92D}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -1279,7 +1296,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1313,83 +1330,83 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>71</v>
-      </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add PostgreSQL datasource and configure Data Asset for activities_sportives table
</commit_message>
<xml_diff>
--- a/docs/dictionnaire_des_donnees.xlsx
+++ b/docs/dictionnaire_des_donnees.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maeva\Documents\OpenClassRoom\P12 - Gérer un projet d'infrastructure\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71D4D01E-903A-4819-8BB8-6007CE314A37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D440EC1C-AAE3-4A31-9803-CBEC8B3C03FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21710" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employes" sheetId="1" r:id="rId1"/>
@@ -219,9 +219,6 @@
     <t>Date de fin de l'activité sportive</t>
   </si>
   <si>
-    <t>duree</t>
-  </si>
-  <si>
     <t>Durée de l'activité en secondes</t>
   </si>
   <si>
@@ -286,6 +283,9 @@
   </si>
   <si>
     <t>adresse_domicile</t>
+  </si>
+  <si>
+    <t>duree_sec</t>
   </si>
 </sst>
 </file>
@@ -355,7 +355,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -372,9 +372,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,7 +813,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B13" t="s">
         <v>28</v>
@@ -838,10 +835,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>79</v>
+      </c>
+      <c r="B15" t="s">
         <v>80</v>
-      </c>
-      <c r="B15" t="s">
-        <v>81</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>16</v>
@@ -861,7 +858,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{89487438-E9F9-4E4A-99B5-90E8A4C27D7E}">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -925,18 +922,18 @@
       <c r="F4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="B5" s="8" t="s">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1055,7 +1052,7 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>46</v>
@@ -1109,8 +1106,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16365D16-3274-4AC6-9B57-6EC96BDEE8BC}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1189,7 @@
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>55</v>
@@ -1207,7 +1204,7 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>59</v>
@@ -1222,7 +1219,7 @@
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>56</v>
@@ -1244,24 +1241,24 @@
     </row>
     <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>61</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="11" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>63</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>16</v>
@@ -1296,7 +1293,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -1345,24 +1342,24 @@
     </row>
     <row r="5" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5" s="4" t="s">
         <v>65</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>66</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>45</v>
@@ -1371,10 +1368,10 @@
     </row>
     <row r="7" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B7" s="4" t="s">
         <v>69</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>70</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>17</v>
@@ -1383,16 +1380,16 @@
     </row>
     <row r="8" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>